<commit_message>
Video name fix and sort by valence
</commit_message>
<xml_diff>
--- a/Video_Summary_Data.xlsx
+++ b/Video_Summary_Data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/memolab/Google Drive/MemoLab/Manuscripts/Video-Norming/paper-videonorming-repo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosecooper/Documents/MemoLab/Manuscripts/Video-Norming/paper-videonorming-repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71AEF64-FC4B-124C-8420-7B751F5E913C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" tabRatio="500"/>
+    <workbookView xWindow="740" yWindow="460" windowWidth="13760" windowHeight="17040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Video Data" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -2147,7 +2148,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -2403,7 +2404,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Table Style 1" defaultPivotStyle="PivotStyleMedium7">
-    <tableStyle name="Table Style 1" pivot="0" count="2">
+    <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2681,12 +2682,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B125" sqref="B125"/>
+      <selection pane="bottomLeft" activeCell="A121" sqref="A121:XFD121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3262,7 +3263,7 @@
         <v>702</v>
       </c>
       <c r="E5" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F5" s="2">
         <v>2011</v>
@@ -5054,7 +5055,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F19" s="2">
         <v>2014</v>
@@ -5694,7 +5695,7 @@
         <v>2</v>
       </c>
       <c r="E24" s="2">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F24" s="2">
         <v>2017</v>
@@ -6206,7 +6207,7 @@
         <v>7</v>
       </c>
       <c r="E28" s="2">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F28" s="2">
         <v>2015</v>
@@ -6334,7 +6335,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F29" s="2">
         <v>2016</v>
@@ -6462,7 +6463,7 @@
         <v>3</v>
       </c>
       <c r="E30" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F30" s="2">
         <v>2017</v>
@@ -7220,7 +7221,7 @@
       <c r="A36" s="23">
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="13" t="s">
         <v>174</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -9918,7 +9919,7 @@
         <v>4</v>
       </c>
       <c r="E57" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F57" s="2">
         <v>2010</v>
@@ -11710,7 +11711,7 @@
         <v>2</v>
       </c>
       <c r="E71" s="2">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F71" s="2">
         <v>2017</v>
@@ -12478,7 +12479,7 @@
         <v>5</v>
       </c>
       <c r="E77" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F77" s="2">
         <v>2015</v>
@@ -13886,7 +13887,7 @@
         <v>0</v>
       </c>
       <c r="E88" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F88" s="2">
         <v>2012</v>
@@ -15550,7 +15551,7 @@
         <v>4</v>
       </c>
       <c r="E101" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F101" s="2">
         <v>2016</v>
@@ -18750,7 +18751,7 @@
         <v>4</v>
       </c>
       <c r="E126" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F126" s="2">
         <v>2017</v>

</xml_diff>

<commit_message>
Updated duration of video #24 from 49 to 51 seconds.
</commit_message>
<xml_diff>
--- a/Video_Summary_Data.xlsx
+++ b/Video_Summary_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosecooper/Documents/MemoLab/Manuscripts/Video-Norming/paper-videonorming-repo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/MemoLab/Manuscripts/Video-Norming/paper-videonorming-repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71AEF64-FC4B-124C-8420-7B751F5E913C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983F9747-AC9D-FB41-A32B-387D6DBCE7E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="460" windowWidth="13760" windowHeight="17040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="740" yWindow="460" windowWidth="13760" windowHeight="16460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Video Data" sheetId="3" r:id="rId1"/>
@@ -2685,9 +2685,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A121" sqref="A121:XFD121"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5823,7 +5823,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="2">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F25" s="2">
         <v>2015</v>
@@ -18995,7 +18995,7 @@
     </row>
     <row r="128" spans="1:42" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sortState ref="A2:AP128">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AP128">
     <sortCondition ref="O2:O128"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>